<commit_message>
Update class support tickets
Update class support tickets
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/IT_Support/ClassPlusSupportTickets.xlsx
+++ b/Offline/BusinessManagement/IT_Support/ClassPlusSupportTickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\IT_Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9C31E5-57AA-4CD0-A0AE-FAB7AFE633DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1806927E-9717-47F1-A092-D9F8FB95E5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>SlNo</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Please Add Co-Admin</t>
+  </si>
+  <si>
+    <t>Cannot Manage Attandence in Batch</t>
   </si>
 </sst>
 </file>
@@ -108,11 +111,9 @@
       <name val="Oxygen"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <name val="Oxygen"/>
     </font>
   </fonts>
   <fills count="3">
@@ -454,7 +455,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,15 +606,31 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1288731</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45211</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Class Plus tickets updated
Class Plus tickets updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/IT_Support/ClassPlusSupportTickets.xlsx
+++ b/Offline/BusinessManagement/IT_Support/ClassPlusSupportTickets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\IT_Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1806927E-9717-47F1-A092-D9F8FB95E5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD903CA8-6F48-4581-B9D8-DAAF13AF9A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>SlNo</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Cannot Manage Attandence in Batch</t>
+  </si>
+  <si>
+    <t>Debashish Nath</t>
+  </si>
+  <si>
+    <t>Issues related to websites</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,6 +472,7 @@
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -519,7 +526,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -544,7 +551,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
@@ -600,7 +607,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -625,7 +632,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
@@ -633,13 +640,27 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1353506</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44934</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>

</xml_diff>